<commit_message>
adicionado politica de preco
</commit_message>
<xml_diff>
--- a/dados/acessorios web.xlsx
+++ b/dados/acessorios web.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,15 +446,25 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>modelo</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>politica</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>full</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>tipo</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>link</t>
         </is>
@@ -471,17 +481,23 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>Modelo identificado mas fora do range de preco</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Classico</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>https://produto.mercadolivre.com.br/MLB-1992683232-fonte-automotiva-60a-jfa-carregador-com-sistema-sci-_JM#position%3D1%26search_layout%3Dstack%26type%3Ditem%26tracking_id%3Dedfb7108-c6d3-4e7b-a86a-c080a604d1b1</t>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>classico</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>https://produto.mercadolivre.com.br/MLB-1992683232-fonte-automotiva-60a-jfa-carregador-com-sistema-sci-_JM#position%3D1%26search_layout%3Dstack%26type%3Ditem%26tracking_id%3D4e91c180-f7d0-4354-88fc-2d08e064eee4</t>
         </is>
       </c>
     </row>
@@ -496,17 +512,23 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>Modelo identificado mas fora do range de preco</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Premium</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>https://produto.mercadolivre.com.br/MLB-2000260510-fonte-automotiva-carregador-jfa-60a-bivolt-automatico-sci-_JM#position%3D2%26search_layout%3Dstack%26type%3Ditem%26tracking_id%3Dedfb7108-c6d3-4e7b-a86a-c080a604d1b1</t>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>premium</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>https://produto.mercadolivre.com.br/MLB-2000260510-fonte-automotiva-carregador-jfa-60a-bivolt-automatico-sci-_JM#position%3D2%26search_layout%3Dstack%26type%3Ditem%26tracking_id%3D4e91c180-f7d0-4354-88fc-2d08e064eee4</t>
         </is>
       </c>
     </row>
@@ -521,17 +543,23 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t>Sem Modelo</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Premium</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>https://produto.mercadolivre.com.br/MLB-1948006562-jfa-k600-controle-longa-distancia-completo-600-metros-_JM#position%3D3%26search_layout%3Dstack%26type%3Ditem%26tracking_id%3Dedfb7108-c6d3-4e7b-a86a-c080a604d1b1</t>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>premium</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>https://produto.mercadolivre.com.br/MLB-1948006562-jfa-k600-controle-longa-distancia-completo-600-metros-_JM#position%3D3%26search_layout%3Dstack%26type%3Ditem%26tracking_id%3D4e91c180-f7d0-4354-88fc-2d08e064eee4</t>
         </is>
       </c>
     </row>
@@ -546,17 +574,27 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>FONTE 70A</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Igual</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Classico</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>https://produto.mercadolivre.com.br/MLB-2191438698-fonte-automotiva-jfa-70a-slim-bivolt-carregador-voltimetro-_JM#position%3D4%26search_layout%3Dstack%26type%3Ditem%26tracking_id%3Dedfb7108-c6d3-4e7b-a86a-c080a604d1b1</t>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>classico</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>https://produto.mercadolivre.com.br/MLB-2191438698-fonte-automotiva-jfa-70a-slim-bivolt-carregador-voltimetro-_JM#position%3D4%26search_layout%3Dstack%26type%3Ditem%26tracking_id%3D4e91c180-f7d0-4354-88fc-2d08e064eee4</t>
         </is>
       </c>
     </row>
@@ -571,17 +609,23 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t>Sem Modelo</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Premium</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>https://produto.mercadolivre.com.br/MLB-3164480798-voltimetro-jfa-vs5hi-3-em-1-sequenciador-high-voltagem-12v-_JM#position%3D5%26search_layout%3Dstack%26type%3Ditem%26tracking_id%3Dedfb7108-c6d3-4e7b-a86a-c080a604d1b1</t>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>premium</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>https://produto.mercadolivre.com.br/MLB-3164480798-voltimetro-jfa-vs5hi-3-em-1-sequenciador-high-voltagem-12v-_JM#position%3D5%26search_layout%3Dstack%26type%3Ditem%26tracking_id%3D4e91c180-f7d0-4354-88fc-2d08e064eee4</t>
         </is>
       </c>
     </row>
@@ -596,17 +640,27 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
+          <t>FONTE 70A</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Igual</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Classico</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>https://produto.mercadolivre.com.br/MLB-1992713167-fonte-carregador-jfa-70a-sistema-inteligente-para-bateria-_JM#position%3D6%26search_layout%3Dstack%26type%3Ditem%26tracking_id%3Dedfb7108-c6d3-4e7b-a86a-c080a604d1b1</t>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>classico</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>https://produto.mercadolivre.com.br/MLB-1992713167-fonte-carregador-jfa-70a-sistema-inteligente-para-bateria-_JM#position%3D6%26search_layout%3Dstack%26type%3Ditem%26tracking_id%3D4e91c180-f7d0-4354-88fc-2d08e064eee4</t>
         </is>
       </c>
     </row>
@@ -621,17 +675,23 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
+          <t>Sem Modelo</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Classico</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>https://produto.mercadolivre.com.br/MLB-1947984228-jfa-k1200-automotivo-controle-longa-distncia-1200-metros-_JM#position%3D7%26search_layout%3Dstack%26type%3Ditem%26tracking_id%3Dedfb7108-c6d3-4e7b-a86a-c080a604d1b1</t>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>classico</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>https://produto.mercadolivre.com.br/MLB-1947984228-jfa-k1200-automotivo-controle-longa-distncia-1200-metros-_JM#position%3D7%26search_layout%3Dstack%26type%3Ditem%26tracking_id%3D4e91c180-f7d0-4354-88fc-2d08e064eee4</t>
         </is>
       </c>
     </row>
@@ -646,17 +706,23 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
+          <t>Sem Modelo</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
+        <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Classico</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>https://produto.mercadolivre.com.br/MLB-3164486838-voltimetro-jfa-vs5hi-3-em-1-sequenciador-high-voltagem-12v-_JM#position%3D8%26search_layout%3Dstack%26type%3Ditem%26tracking_id%3Dedfb7108-c6d3-4e7b-a86a-c080a604d1b1</t>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>classico</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>https://produto.mercadolivre.com.br/MLB-3164486838-voltimetro-jfa-vs5hi-3-em-1-sequenciador-high-voltagem-12v-_JM#position%3D8%26search_layout%3Dstack%26type%3Ditem%26tracking_id%3D4e91c180-f7d0-4354-88fc-2d08e064eee4</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
mudei para entrar na planilha
</commit_message>
<xml_diff>
--- a/dados/acessorios web.xlsx
+++ b/dados/acessorios web.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,35 +436,45 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>data</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>loja</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>nome</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>modelo</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>preco</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>politica</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>full</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>tipo</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>link</t>
         </is>
@@ -473,272 +483,352 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>30/07/2024</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>acessorios web</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>Fonte Automotiva 60a Jfa Carregador Com Sistema Sci</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>FONTE 60A STORM</t>
         </is>
       </c>
-      <c r="C2" t="n">
+      <c r="E2" t="n">
         <v>369.95</v>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>Baixo</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>classico</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>https://produto.mercadolivre.com.br/MLB-1992683232-fonte-automotiva-60a-jfa-carregador-com-sistema-sci-_JM#position%3D1%26search_layout%3Dstack%26type%3Ditem%26tracking_id%3Df58cbb8f-93eb-4efd-b58f-a6d1e4dca198</t>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>https://produto.mercadolivre.com.br/MLB-1992683232-fonte-automotiva-60a-jfa-carregador-com-sistema-sci-_JM#position%3D1%26search_layout%3Dstack%26type%3Ditem%26tracking_id%3D0665459a-e415-4da0-a7c8-7b68af51a563</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>30/07/2024</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>acessorios web</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>Fonte Automotiva Jfa 70a Slim Bivolt Carregador Voltímetro</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>FONTE 70A STORM</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="E3" t="n">
         <v>493.42</v>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>Igual</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>classico</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>https://produto.mercadolivre.com.br/MLB-2191438698-fonte-automotiva-jfa-70a-slim-bivolt-carregador-voltimetro-_JM#position%3D2%26search_layout%3Dstack%26type%3Ditem%26tracking_id%3Df58cbb8f-93eb-4efd-b58f-a6d1e4dca198</t>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>https://produto.mercadolivre.com.br/MLB-2191438698-fonte-automotiva-jfa-70a-slim-bivolt-carregador-voltimetro-_JM#position%3D2%26search_layout%3Dstack%26type%3Ditem%26tracking_id%3D0665459a-e415-4da0-a7c8-7b68af51a563</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>30/07/2024</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>acessorios web</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>Jfa K1200 Automotivo - Controle Longa Distância 1200 Metros</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>K1200</t>
         </is>
       </c>
-      <c r="C4" t="n">
+      <c r="E4" t="n">
         <v>59.9</v>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>Baixo</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>classico</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>https://produto.mercadolivre.com.br/MLB-1947984228-jfa-k1200-automotivo-controle-longa-distncia-1200-metros-_JM#position%3D3%26search_layout%3Dstack%26type%3Ditem%26tracking_id%3Df58cbb8f-93eb-4efd-b58f-a6d1e4dca198</t>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>https://produto.mercadolivre.com.br/MLB-1947984228-jfa-k1200-automotivo-controle-longa-distncia-1200-metros-_JM#position%3D3%26search_layout%3Dstack%26type%3Ditem%26tracking_id%3D0665459a-e415-4da0-a7c8-7b68af51a563</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>30/07/2024</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>acessorios web</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>Fonte Automotiva Carregador Jfa 60a Bivolt Automático Sci</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>FONTE 60A STORM</t>
         </is>
       </c>
-      <c r="C5" t="n">
+      <c r="E5" t="n">
         <v>434.77</v>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>Baixo</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>premium</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>https://produto.mercadolivre.com.br/MLB-2000260510-fonte-automotiva-carregador-jfa-60a-bivolt-automatico-sci-_JM#position%3D4%26search_layout%3Dstack%26type%3Ditem%26tracking_id%3Df58cbb8f-93eb-4efd-b58f-a6d1e4dca198</t>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>https://produto.mercadolivre.com.br/MLB-2000260510-fonte-automotiva-carregador-jfa-60a-bivolt-automatico-sci-_JM#position%3D4%26search_layout%3Dstack%26type%3Ditem%26tracking_id%3D0665459a-e415-4da0-a7c8-7b68af51a563</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>30/07/2024</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>acessorios web</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
           <t>Voltímetro Jfa Vs5hi 3 Em 1 Sequenciador High Voltagem 12v</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>Sem Modelo</t>
         </is>
       </c>
-      <c r="C6" t="n">
+      <c r="E6" t="n">
         <v>67.38</v>
       </c>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>premium</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>https://produto.mercadolivre.com.br/MLB-3164480798-voltimetro-jfa-vs5hi-3-em-1-sequenciador-high-voltagem-12v-_JM#position%3D5%26search_layout%3Dstack%26type%3Ditem%26tracking_id%3Df58cbb8f-93eb-4efd-b58f-a6d1e4dca198</t>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>https://produto.mercadolivre.com.br/MLB-3164480798-voltimetro-jfa-vs5hi-3-em-1-sequenciador-high-voltagem-12v-_JM#position%3D5%26search_layout%3Dstack%26type%3Ditem%26tracking_id%3D0665459a-e415-4da0-a7c8-7b68af51a563</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>30/07/2024</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>acessorios web</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>Fonte Carregador Jfa 70a Sistema Inteligente Para Bateria</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>FONTE 70A STORM</t>
         </is>
       </c>
-      <c r="C7" t="n">
+      <c r="E7" t="n">
         <v>493.42</v>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>Igual</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="H7" t="inlineStr">
         <is>
           <t>classico</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>https://produto.mercadolivre.com.br/MLB-1992713167-fonte-carregador-jfa-70a-sistema-inteligente-para-bateria-_JM#position%3D6%26search_layout%3Dstack%26type%3Ditem%26tracking_id%3Df58cbb8f-93eb-4efd-b58f-a6d1e4dca198</t>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>https://produto.mercadolivre.com.br/MLB-1992713167-fonte-carregador-jfa-70a-sistema-inteligente-para-bateria-_JM#position%3D6%26search_layout%3Dstack%26type%3Ditem%26tracking_id%3D0665459a-e415-4da0-a7c8-7b68af51a563</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>30/07/2024</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>acessorios web</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
           <t>Jfa K600 - Controle Longa Distancia Completo 600 Metros</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>K600</t>
         </is>
       </c>
-      <c r="C8" t="n">
+      <c r="E8" t="n">
         <v>61.98</v>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>Baixo</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>premium</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>https://produto.mercadolivre.com.br/MLB-1948006562-jfa-k600-controle-longa-distancia-completo-600-metros-_JM#position%3D7%26search_layout%3Dstack%26type%3Ditem%26tracking_id%3Df58cbb8f-93eb-4efd-b58f-a6d1e4dca198</t>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>https://produto.mercadolivre.com.br/MLB-1948006562-jfa-k600-controle-longa-distancia-completo-600-metros-_JM#position%3D7%26search_layout%3Dstack%26type%3Ditem%26tracking_id%3D0665459a-e415-4da0-a7c8-7b68af51a563</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>30/07/2024</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>acessorios web</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
           <t>Voltímetro Jfa Vs5hi 3 Em 1 Sequenciador High Voltagem 12v</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>Sem Modelo</t>
         </is>
       </c>
-      <c r="C9" t="n">
+      <c r="E9" t="n">
         <v>67.37</v>
       </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr">
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="H9" t="inlineStr">
         <is>
           <t>classico</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>https://produto.mercadolivre.com.br/MLB-3164486838-voltimetro-jfa-vs5hi-3-em-1-sequenciador-high-voltagem-12v-_JM#position%3D8%26search_layout%3Dstack%26type%3Ditem%26tracking_id%3Df58cbb8f-93eb-4efd-b58f-a6d1e4dca198</t>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>https://produto.mercadolivre.com.br/MLB-3164486838-voltimetro-jfa-vs5hi-3-em-1-sequenciador-high-voltagem-12v-_JM#position%3D8%26search_layout%3Dstack%26type%3Ditem%26tracking_id%3D0665459a-e415-4da0-a7c8-7b68af51a563</t>
         </is>
       </c>
     </row>

</xml_diff>